<commit_message>
use case test visualization
</commit_message>
<xml_diff>
--- a/2023-2024/jiaqi-li/analyse/pages_data.xlsx
+++ b/2023-2024/jiaqi-li/analyse/pages_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook/Documents/GitHub/student-projects/2023-2024/jiaqi-li/analyse/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5130AF19-53FB-5A48-87FD-54FE034D10F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB5436F3-44A8-BD45-A596-AE943D0E2897}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4820" yWindow="880" windowWidth="25420" windowHeight="17000" activeTab="1" xr2:uid="{6FAD5CCA-AC59-CA4E-9096-0B75BAA124B0}"/>
+    <workbookView xWindow="4820" yWindow="880" windowWidth="25420" windowHeight="17000" activeTab="2" xr2:uid="{6FAD5CCA-AC59-CA4E-9096-0B75BAA124B0}"/>
   </bookViews>
   <sheets>
     <sheet name="bert-base-uncased_30522" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="64">
   <si>
     <t>URL</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -828,9 +828,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>https://blog.dataiku.com/large-language-model-chatgpt</t>
-  </si>
-  <si>
     <t>What Is a Large Language Model, the Tech Behind ChatGPT?</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -3662,23 +3659,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>[-0.07667841762304306,-0.03638090938329697,0.014749150723218918,0.004683269187808037,0.0170003529638052,-0.06924188137054443,0.058084405958652496,0.02414003200829029,0.04539569839835167,-0.018142927438020706,-0.0074715702794492245,0.045392945408821106,-0.0195564404129982,-0.001471954514272511,0.1053355261683464,0.03991313651204109,0.05364614725112915,-0.058959804475307465,-0.011084681376814842,-0.08514078706502914,0.03844103217124939,0.08514857292175293,0.0849657952785492,0.0058989147655665874,0.029208268970251083,0.039262618869543076,-0.040660399943590164,-0.05273155868053436,0.04206586629152298,0.025186877697706223,0.023351866751909256,0.07716766744852066,0.08064793050289154,0.04946430027484894,-0.07355114817619324,0.01811332069337368,-0.04535223916172981,-0.0029889976140111685,-0.014694076962769032,-0.0010332217207178473,-0.02582705207169056,-0.06100766360759735,0.047281455248594284,0.029642531648278236,0.04510573670268059,-0.013010748662054539,-0.07961755990982056,0.04197107255458832,-0.017225679010152817,0.02465868927538395,-0.09299693256616592,-0.04495999589562416,0.05796594172716141,-0.0028036872390657663,0.005418022163212299,0.042729053646326065,-0.05052686110138893,0.025713741779327393,0.044057197868824005,-0.033004000782966614,0.0022612246684730053,0.004590920638293028,0.006602018140256405,-0.013227366842329502,-0.004845679737627506,-0.023301556706428528,0.016284579411149025,0.0180077962577343,0.02576330676674843,-0.09181661903858185,0.039992887526750565,0.04828967899084091,0.0021234056912362576,0.03186837211251259,-0.05227413773536682,0.08927489817142487,0.025311458855867386,-0.009033064357936382,-0.0010995934717357159,0.0011692183325067163,0.0514332577586174,-0.028737377375364304,0.06329159438610077,0.022734422236680984,-0.03900265321135521,0.005095052532851696,0.05627194046974182,0.06597094237804413,0.0229636337608099,0.03149816021323204,-0.043188586831092834,-0.0333520770072937,0.09416307508945465,0.0311959907412529,-0.09127578139305115,-0.056115031242370605,-0.019978541880846024,-0.026161136105656624,-0.04137115180492401,0.06550854444503784,-0.009022620506584644,-0.02232631854712963,-0.0013719352427870035,-0.018741119652986526,-0.05811237171292305,-0.039768919348716736,0.06965557485818863,-0.011001846753060818,0.03759339451789856,-0.049794647842645645,-0.024673625826835632,-0.10667029768228531,0.06781766563653946,-0.04080716893076897,0.0001946979173226282,0.0462469756603241,-0.06567074358463287,0.026272635906934738,0.03195571154356003,0.08035881072282791,0.022318046540021896,-0.04296533018350601,-0.04700752720236778,0.008319267071783543,0.013279257342219353,0.054609257727861404,0.03060043975710869,-4.251463683206739e-34,0.05951463058590889,-0.0060077547095716,0.016108309850096703,0.05736605077981949,0.020561859011650085,0.049154698848724365,-0.05880775302648544,-0.04160696268081665,-0.027100944891572,-0.0598418228328228,-0.06121092289686203,-0.040792159736156464,-0.039958421140909195,0.0692238137125969,0.04846620932221413,-0.06246962398290634,-0.026753047481179237,0.05672356113791466,0.0919456034898758,0.021743325516581535,-0.01251957006752491,0.017658237367868423,0.05086573213338852,0.01823372207581997,0.03891657665371895,0.0927201434969902,0.03351765498518944,-0.1136145070195198,0.07264164090156555,0.026713434606790543,-0.05633106455206871,0.022355079650878906,-0.04439437389373779,0.04070892557501793,-0.015094886533915997,-0.007746755611151457,-0.0652807429432869,-0.09256529062986374,-0.01818581484258175,0.05399180203676224,-0.0418575145304203,-0.014982357621192932,-0.02049526758491993,-0.08606411516666412,-0.0004693965020123869,-0.009975243359804153,-0.05820697918534279,0.01650102809071541,0.01433198619633913,-0.0022262868005782366,-0.06782088428735733,0.07145649194717407,-0.04133720323443413,0.015447462908923626,0.09834972023963928,-0.11559484153985977,0.013701741583645344,-0.035305205732584,0.03800931200385094,0.042052190750837326,-0.06326029449701309,-0.035218749195337296,-0.0157861839979887,-0.02731514535844326,0.04391210898756981,0.021024266257882118,0.04603581130504608,-0.032524045556783676,0.017220478504896164,0.013229788281023502,0.009739520028233528,0.012381402775645256,-0.042932573705911636,0.01526376511901617,-0.060894060879945755,0.06104506924748421,0.040969327092170715,-0.0026730543468147516,0.055545687675476074,-0.0045267269015312195,-0.06703812628984451,-0.04869433119893074,0.00863763876259327,-0.042989615350961685,0.008121825754642487,-0.010621722787618637,-0.0016196916112676263,-0.009066233411431313,0.029983125627040863,0.05621710792183876,-0.11803771555423737,-0.038279611617326736,-0.07558278739452362,0.0582946240901947,0.03342491388320923,8.90700997799337e-34,-0.10502943396568298,0.05357155576348305,-0.1181967481970787,0.06370294839143753,-0.04221704974770546,-0.07914136350154877,0.028171708807349205,0.07436063885688782,0.03205323591828346,0.031331442296504974,-0.040158845484256744,-0.02018987014889717,0.07767301052808762,-0.02078329585492611,0.07827267795801163,-0.08116547763347626,0.046150993555784225,-0.07237506657838821,-0.05606810376048088,0.034544941037893295,-0.00008787145634414628,-0.005410830955952406,-0.10937096923589706,-0.030462488532066345,0.0821802094578743,0.01961171254515648,-0.02152646705508232,-0.0010001118062064052,-0.03239632770419121,-0.008812589570879936,0.03100505843758583,0.04218531772494316,-0.06623171269893646,0.029363805428147316,0.04670197144150734,0.025853443890810013,0.1279490441083908,0.015064690262079239,-0.051594216376543045,0.01932067982852459,0.1178525909781456,0.0173622015863657,-0.07034663110971451,-0.013867763802409172,-0.042570337653160095,0.03908883407711983,-0.11333081126213074,0.006868002470582724,-0.041408784687519073,-0.009113872423768044,0.03748269006609917,-0.04891936480998993,0.06482700258493423,-0.11880546063184738,-0.02295673079788685,-0.062451690435409546,0.005855101626366377,0.024848420172929764,-0.06466817110776901,-0.015075725503265858,-0.02972905896604061,-0.06723585724830627,0.06949804723262787,-0.01929991878569126,-0.021487586200237274,-0.038917332887649536,0.050349000841379166,0.07610911130905151,0.03221549093723297,-0.06638509780168533,0.052932918071746826,-0.10322912782430649,-0.02549554780125618,0.10439690202474594,0.004070222843438387,0.06442692875862122,-0.015204653143882751,-0.0181723665446043,0.004965391010046005,-0.058568716049194336,0.06141982972621918,-0.009263302199542522,0.08760014921426773,0.05239364132285118,0.10489729046821594,0.0258632842451334,0.021032152697443962,0.046656981110572815,0.05777750536799431,0.06710830330848694,-0.05425269156694412,0.09034911543130875,-0.08300046622753143,0.13901272416114807,-0.016199367120862007,-3.510633916903316e-8,-0.02846583165228367,-0.1259508579969406,-0.03951422870159149,0.08225399255752563,0.005607113242149353,0.008836892433464527,-0.012365331873297691,-0.0021822659764438868,0.005471786949783564,0.009217941202223301,0.008958129212260246,-0.002817853819578886,-0.08059968054294586,-0.0395401194691658,0.06695972383022308,0.044778626412153244,-0.0024724039249122143,-0.043379541486501694,0.005801560822874308,-0.0723244771361351,0.04168954864144325,-0.025092409923672676,0.04817634075880051,0.006940648891031742,-0.08907290548086166,-0.0708964616060257,-0.05567658320069313,0.039759159088134766,-0.0629970133304596,-0.002179404953494668,0.06146171689033508,-0.025236647576093674,0.04841456189751625,0.020176351070404053,0.06887723505496979,0.03344375267624855,-0.05339594930410385,-0.03092830628156662,0.07225744426250458,0.007299492135643959,0.01978272944688797,0.03166785091161728,-0.04205489531159401,-0.040466949343681335,-0.012782412581145763,-0.05384206026792526,-0.04470634460449219,-0.15385495126247406,-0.015221551060676575,-0.05983641743659973,-0.07799850404262543,-0.010617001913487911,0.022645097225904465,0.03730546310544014,0.10717885941267014,-0.014171699061989784,0.034345563501119614,-0.01571812853217125,0.015269213356077671,0.030568866059184074,-0.030597025528550148,0.07619443535804749,0.06999038904905319,-0.020719973370432854
- embedding for page content-0.06116609275341034,-0.10362809896469116,0.061865486204624176,-0.02133701555430889,-0.01165072899311781,-0.03117717057466507,-0.02056298404932022,0.039986733347177505,0.13929420709609985,0.026935352012515068,-0.06930243968963623,0.03605935722589493,0.01470204908400774,-0.018420981243252754,-0.03142170608043671,0.020945914089679718,0.042031336575746536,-0.014423503540456295,-0.1240803450345993,-0.06777589023113251,0.10982134193181992,0.02897101640701294,-0.03674370050430298,-0.0011521324049681425,-0.008563676849007607,0.055655285716056824,-0.022724760696291924,-0.045631613582372665,-0.04172731563448906,0.021891143172979355,0.020002126693725586,0.07756317406892776,0.036617569625377655,0.1214192807674408,-0.1084785908460617,0.06637874990701675,-0.03631625324487686,-0.0025904832873493433,0.031064221635460854,-0.009514766745269299,0.0014779835473746061,-0.02534586191177368,0.04721919074654579,-0.01460468303412199,0.13851264119148254,-0.016714246943593025,-0.07200255990028381,-0.018286598846316338,-0.07883622497320175,-0.022874047979712486,-0.12998780608177185,-0.0297701358795166,-0.0183385219424963,0.10580720752477646,-0.008686580695211887,-0.016031324863433838,0.009642405435442924,0.04612681642174721,-0.081243596971035,-0.009970854967832565,-0.02252558432519436,-0.06568082422018051,-0.0027834298089146614,-0.030169649049639702,0.039654165506362915,-0.00361393834464252,-0.02937161736190319,0.04831146448850632,0.009825128130614758,-0.07906340062618256,0.05147041380405426,-0.005120421759784222,0.005684060975909233,0.04011170566082001,0.026496781036257744,-0.0032447255216538906,0.1040564626455307,0.04301612451672554,0.07195809483528137,-0.019713647663593292,0.02477951906621456,0.041543398052453995,0.055080026388168335,-0.015376797877252102,0.018918374553322792,-0.017536316066980362,0.02951747179031372,0.0322679728269577,-0.019840246066451073,0.007000465411692858,-0.07752492278814316,-0.07792247831821442,-0.04913656786084175,-0.0010249025654047728,0.07343226671218872,-0.008226806297898293,0.007884170860052109,-0.019108399748802185,-0.004591973498463631,0.04565611109137535,0.025660835206508636,0.02270014025270939,0.0537758506834507,-0.0740802064538002,-0.02802271768450737,0.0004128070140723139,0.02538895420730114,0.031335361301898956,0.04739634692668915,-0.0880219042301178,-0.08512089401483536,0.03383351117372513,0.0025027557276189327,0.04551291838288307,0.023647364228963852,-0.06448206305503845,0.0325963981449604,0.008644666522741318,0.012087143026292324,0.06356646120548248,-0.046456824988126755,0.02118898183107376,-0.02556261233985424,-0.01675792597234249,0.005512076895684004,0.007825731299817562,-0.07104139029979706,4.737000522787931e-33,0.01839081011712551,-0.01312713697552681,-0.005626991391181946,0.10100676864385605,0.06009911000728607,-0.009300656616687775,0.016027461737394333,-0.002664115047082305,0.03351111710071564,0.02631002478301525,-0.07533098757266998,0.08064620196819305,0.004881351254880428,0.13627950847148895,0.06121669337153435,-0.025043949484825134,-0.060823507606983185,-0.034774746745824814,0.06505738943815231,-0.08994559943675995,0.01643151231110096,0.043557118624448776,0.0694757029414177,-0.012328505516052246,-0.012497887015342712,0.029574738815426826,0.045144837349653244,-0.10511814802885056,-0.07070957124233246,0.002043228829279542,-0.10087533295154572,0.01672651618719101,0.003262605518102646,-0.01577184908092022,0.002929207170382142,-0.021208476275205612,0.026849623769521713,-0.08066045492887497,0.061364538967609406,-0.045945100486278534,-0.01629643514752388,-0.01262833084911108,-0.013728102669119835,-0.03667210042476654,-0.034102167934179306,-0.0037185170222073793,-0.030476810410618782,-0.030352981761097908,-0.004445664118975401,-0.0663575679063797,0.03580116108059883,-0.027972690761089325,-0.032896000891923904,-0.00104001525323838,0.07131006568670273,0.024327881634235382,-0.017307648435235023,0.0380784347653389,0.04602384939789772,0.09919526427984238,-0.023658905178308487,0.0179037693887949,-0.022931525483727455,0.077882781624794,0.13203522562980652,-0.006354125682264566,-0.04624854028224945,0.04586830362677574,0.08212806284427643,-0.007594216149300337,0.010619085282087326,0.012635419145226479,-0.005656160414218903,-0.040407776832580566,-0.045349981635808945,0.010169187560677528,-0.0033463239669799805,-0.04864699766039848,-0.03275413066148758,0.104361891746521,-0.05324206128716469,-0.02813699096441269,0.0028537113685160875,-0.08675169944763184,-0.01953939162194729,0.020367955788969994,0.026330146938562393,-0.03247823938727379,0.009892112575471401,-0.04813142865896225,-0.03604124113917351,-0.040607210248708725,0.013847438618540764,0.0025548262055963278,0.03881459683179855,-5.759732403223154e-33,-0.08020413666963577,0.027714546769857407,-0.15791793167591095,0.08225297927856445,0.005006690043956041,-0.0760977491736412,-0.03134744614362717,0.04463624581694603,-0.102743960916996,-0.010484096594154835,-0.042181164026260376,-0.03140193596482277,0.07723285257816315,-0.016835609450936317,0.05829247459769249,-0.06380058825016022,0.0073593491688370705,-0.06176741048693657,0.012742772698402405,0.03452404588460922,0.01779480092227459,0.06751563400030136,-0.13069134950637817,-0.014572081156075,-0.024406347423791885,-0.0027903602458536625,-0.08549214154481888,0.08862386643886566,-0.011404089629650116,0.04655182734131813,0.04949890077114105,-0.04304074868559837,-0.06568504869937897,0.026300989091396332,0.0016234962968155742,0.06128504499793053,0.09946822375059128,-0.06074416637420654,-0.0009922313038259745,-0.03875399008393288,0.04105374962091446,-0.051318828016519547,-0.032431721687316895,-0.04954056441783905,-0.012657180428504944,-0.0038779289461672306,-0.1087423712015152,-0.014196290634572506,-0.039018526673316956,-0.011429480277001858,0.08749283850193024,-0.0342203713953495,0.01838637888431549,-0.07494800537824631,-0.06907643377780914,-0.05959992855787277,-0.008444566279649734,-0.0191542636603117,0.0248250812292099,-0.020584536716341972,-0.018695097416639328,-0.09131696075201035,0.06834477186203003,-0.026461536064743996,-0.0443015918135643,0.006047695875167847,-0.02941957116127014,0.012984606437385082,0.0030260165221989155,-0.02506340481340885,0.04779866710305214,0.008353731594979763,0.02924150787293911,0.06788616627454758,-0.018982624635100365,-0.006497182417660952,-0.019901132211089134,-0.023851947858929634,0.0019382750615477562,-0.10148942470550537,-0.010148152709007263,-0.029516184702515602,0.036008115857839584,0.030096137896180153,0.08100063353776932,0.017910175025463104,0.019940540194511414,0.08355323225259781,0.010298280045390129,-0.010086078196763992,0.023010024800896645,0.026226656511425972,-0.044183116406202316,0.03915645554661751,-0.06892623752355576,-5.810201386680092e-8,-0.03024064376950264,-0.04660952091217041,-0.016626223921775818,0.026923807337880135,0.052000805735588074,-0.08056408166885376,0.058120086789131165,0.07876017689704895,-0.01787634938955307,0.031082607805728912,0.0471491813659668,0.0022755011450499296,-0.06318596005439758,-0.014174817129969597,0.07823559641838074,0.10196462273597717,0.028522364795207977,-0.03981582447886467,0.011663819663226604,-0.05036488175392151,0.07273859530687332,-0.03333786502480507,-0.03953150287270546,0.0651405081152916,0.08337312936782837,-0.07905169576406479,-0.0627569779753685,0.05382382497191429,-0.08418389409780502,0.03515284135937691,0.00592394545674324,-0.0064392718486487865,-0.0383361354470253,0.02957613579928875,0.08413852006196976,0.07191785424947739,0.07082310318946838,-0.10317006707191467,0.00507113104686141,-0.04318613559007645,0.004206089768558741,0.005464851390570402,-0.016039051115512848,0.005375828593969345,0.052773330360651016,-0.06545157730579376,-0.03813861683011055,-0.12479016929864883,0.004423332400619984,0.026491302996873856,-0.01697634533047676,0.06319067627191544,-0.026647185906767845,0.011838392354547977,-0.0014748233370482922,-0.011111389845609665,0.01275655161589384,-0.047415852546691895,0.007086853962391615,0.034578610211610794,0.014022220857441425,0.14679095149040222,0.044199537485837936,-0.022492485120892525]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>[--0.08861415833234787,-0.0416453517973423,-0.015285965986549854,-0.031236819922924042,-0.033545151352882385,-0.07572811096906662,-0.10687108337879181,0.03258390724658966,-0.03055522032082081,-0.061724480241537094,-0.0868893712759018,0.01353105716407299,-0.0398903526365757,-0.020236173644661903,0.0008984606829471886,-0.0006998720346018672,-0.01256787683814764,0.032651323825120926,-0.09016240388154984,-0.08588181436061859,0.0677943155169487,0.07395553588867188,-0.047948818653821945,0.028694458305835724,-0.05736779421567917,0.004636651836335659,0.00591965252533555,-0.006066696252673864,-0.02472926862537861,0.006809897720813751,-0.03353552147746086,-0.0588238462805748,-0.045347586274147034,0.04337560757994652,-0.05396323278546333,0.05274508520960808,0.10195180773735046,0.0046644131653010845,-0.005802451632916927,-0.01412081066519022,-0.003974903840571642,-0.08620896935462952,-0.042115408927202225,-0.03712967410683632,0.05351204052567482,-0.026932811364531517,-0.07879295200109482,-0.17889705300331116,-0.06903326511383057,0.03425119072198868,-0.03597957640886307,-0.07212844491004944,-0.06990452855825424,0.04909346252679825,-0.04596942663192749,0.05464037507772446,0.055095043033361435,0.0012528729857876897,-0.042321473360061646,-0.051551371812820435,-0.05317028611898422,-0.061922501772642136,0.007018471602350473,0.0801953375339508,-0.02182837948203087,-0.016811922192573547,-0.0007797287544235587,0.004563171416521072,0.1129416674375534,-0.07983756810426712,-0.036265794187784195,0.012442623265087605,-0.021289536729454994,0.015719473361968994,-0.008191955275833607,0.0005369919235818088,0.0716916024684906,0.05802719667553902,0.010085883550345898,-0.013016822747886181,-0.03149092197418213,0.0008126820903271437,0.03391913324594498,0.0351218655705452,-0.0012321402318775654,0.09957783669233322,-0.03473298251628876,0.01759064383804798,-0.006292752921581268,-0.010538148693740368,-0.07222137600183487,-0.06961370259523392,0.06497926265001297,0.024056436493992805,-0.04321344196796417,0.019089121371507645,-0.022440992295742035,-0.0606020987033844,0.05867739021778107,0.02050013095140457,-0.10296349972486496,0.0010142280953004956,0.05314956605434418,-0.04463727027177811,-0.0054864464327692986,-0.005001158453524113,-0.06561466306447983,0.0008229342056438327,-0.015629954636096954,-0.10465411841869354,-0.010522997938096523,-0.07345084846019745,-0.03836608678102493,-0.03453730046749115,0.05854957550764084,0.011030161753296852,-0.06866592168807983,-0.060371801257133484,-0.043643802404403687,0.10413865000009537,-0.07586723566055298,-0.00677602831274271,0.010421248152852058,-0.004999800585210323,0.018629400059580803,-0.03386705741286278,-0.07112549245357513,-2.5207098820941586e-33,0.013758925721049309,-0.07242990285158157,0.04763162136077881,-0.02728687971830368,0.11022943258285522,-0.0038848603144288063,0.07208802551031113,0.014302851632237434,-0.07304053008556366,0.007392518687993288,0.02348690666258335,0.05164490267634392,-0.012890974059700966,0.06742703914642334,-0.026047799736261368,-0.008445088751614094,-0.03674953430891037,0.05177466943860054,-0.023166967555880547,0.019007643684744835,0.014282935298979282,0.08918444812297821,0.0029961951076984406,0.004966838285326958,0.06445526331663132,-0.032637789845466614,0.05134573578834534,0.03599756956100464,-0.07789025455713272,0.037986088544130325,-0.00034893411793746054,-0.02653220109641552,0.032696306705474854,-0.05813044309616089,0.001452227937988937,0.0035141934640705585,0.04209515452384949,0.033978287130594254,0.019025545567274094,-0.02875804528594017,0.029954198747873306,-0.0010368252405896783,0.020446037873625755,-0.025818511843681335,-0.04999670758843422,0.0006745914579369128,-0.052610501646995544,-0.04814746603369713,-0.013064569793641567,-0.01145867072045803,0.04226132109761238,-0.02357134036719799,0.062217872589826584,0.02158433385193348,0.03960482403635979,-0.055696040391922,0.03568805754184723,0.06762305647134781,0.0030761242378503084,0.005637252703309059,-0.0003492495743557811,0.044130146503448486,-0.007610798347741365,0.0826956108212471,-0.020507361739873886,0.0003651201259344816,0.03904897719621658,0.04302101582288742,0.05530036240816116,0.05925678834319115,0.006584573537111282,0.07746513932943344,-0.0499606654047966,0.02054445818066597,0.09567726403474808,-0.009975663386285305,0.03237108513712883,-0.017686204984784126,-0.039641834795475006,0.05650966241955757,-0.05990104377269745,0.023806730285286903,0.021921910345554352,0.008154737763106823,-0.06014057993888855,0.07935377210378647,-0.044360142201185226,-0.003782201325520873,0.006763943005353212,-0.0003828492190223187,-0.09389795362949371,0.000054601892770733684,-0.05495423823595047,0.054075781255960464,0.03652456775307655,-1.7999812348263972e-33,0.090720996260643,0.09758063405752182,-0.07674086838960648,0.10562846809625626,0.004586813505738974,0.017922764644026756,-0.0002830916200764477,-0.06786663085222244,-0.022855618968605995,0.021228056401014328,-0.03355248272418976,0.1072133257985115,0.029428629204630852,0.08279737830162048,0.034095000475645065,-0.07068140804767609,-0.11346441507339478,-0.17287881672382355,0.0354776531457901,-0.0022358535788953304,-0.03799431025981903,0.02483353205025196,-0.02319561317563057,-0.018046550452709198,-0.03456777334213257,-0.01572038233280182,-0.1602235585451126,0.01973070576786995,0.04674682393670082,0.00009814972872845829,-0.026997599750757217,-0.011161626316606998,0.025988390669226646,-0.09159308671951294,-0.10149852931499481,0.06374502927064896,0.02326209470629692,0.03570591285824776,0.11226183921098709,-0.012813873589038849,-0.04926786199212074,-0.043155983090400696,0.025612110272049904,-0.07972483336925507,-0.09115728735923767,0.04140958935022354,0.10224860906600952,0.006081623025238514,-0.034435804933309555,-0.05353683978319168,-0.03457590565085411,0.06834147870540619,-0.02500440925359726,0.05432803928852081,0.009177790023386478,0.021600352600216866,-0.025098955258727074,0.0035928827710449696,-0.09587088227272034,0.017864150926470757,-0.016726769506931305,0.030506322160363197,0.03253728151321411,0.04285847395658493,-0.0837063416838646,0.005900312215089798,-0.025416040793061256,-0.02105499804019928,-0.003458706894889474,-0.020637670531868935,0.009767448529601097,-0.0011290267575532198,-0.022551631554961205,0.06482832133769989,-0.022782811895012856,-0.0642748773097992,-0.04789303243160248,-0.00007090232247719541,0.010205984115600586,0.07964382320642471,-0.014162492007017136,-0.015352866612374783,0.0002947983448393643,0.10473450273275375,0.1088242307305336,-0.038245789706707,0.08964421600103378,-0.019832724705338478,0.004042681772261858,-0.02960776351392269,0.01737804338335991,0.07548071444034576,-0.08385809510946274,-0.00756809301674366,-0.03056159056723118,-3.254081804016096e-8,0.0028776731342077255,0.03218218684196472,0.05953732505440712,0.059806421399116516,-0.023162154480814934,-0.012764208018779755,0.01997974142432213,0.1640552282333374,0.0035036078188568354,0.03133802488446236,0.0019289960619062185,-0.014055952429771423,-0.021145693957805634,0.0153757743537426,0.030150674283504486,0.06827739626169205,0.03570759668946266,0.0390823669731617,0.0035134884528815746,-0.005935993976891041,0.019441552460193634,-0.03830980509519577,0.008445159532129765,-0.012935638427734375,-0.028229134157299995,-0.056522585451602936,0.05233171954751015,0.0075251078233122826,-0.01999911107122898,0.011988567188382149,-0.08123207092285156,0.020788805559277534,-0.019000766798853874,-0.04794834926724434,0.1459568589925766,0.07134490460157394,-0.01870449259877205,-0.0384332649409771,-0.016004623845219612,0.018292609602212906,0.025270944461226463,-0.04467513784766197,0.01622607558965683,0.00005706916272174567,-0.01431744359433651,0.061732739210128784,0.007022933103144169,-0.04232361167669296,-0.029704125598073006,0.06466051936149597,-0.058940988034009933,0.031334418803453445,-0.019404256716370583,0.06287102401256561,-0.006035404745489359,0.04396717622876167,0.05071181803941727,-0.12261836230754852,-0.008913788944482803,0.03406069427728653,0.01285090297460556,0.06872457265853882,0.08229980617761612,-0.041040051728487015]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>[-0.1443004012107849,-0.05591548606753349,0.01067250408232212,0.02434355393052101,-0.03345674276351929,-0.02363518811762333,-0.00017077427764888853,0.045953355729579926,-0.009510498493909836,-0.0492122545838356,-0.05248343199491501,-0.07560040801763535,-0.03752075135707855,0.006882817018777132,0.038184065371751785,0.03680780529975891,0.03739960491657257,0.019740335643291473,-0.16256944835186005,-0.06503906846046448,0.1485968977212906,0.07554468512535095,-0.009658623486757278,-0.032088860869407654,-0.012750323861837387,0.013647220097482204,-0.03475861996412277,-0.06344331800937653,-0.0068017407320439816,0.00940051767975092,-0.014478025957942009,-0.020417911931872368,-0.047344405204057693,0.0863724872469902,-0.01779685728251934,0.050724368542432785,0.029098719358444214,-0.008487282320857048,0.005789230577647686,-0.05033349245786667,-0.03621708229184151,-0.035252299159765244,-0.07515218108892441,-0.06184951215982437,0.05485881119966507,-0.08334758877754211,-0.06971399486064911,-0.1523135006427765,-0.04892782121896744,-0.0012957097496837378,-0.06741610914468765,-0.021908914670348167,0.0005195013945922256,0.04274344816803932,-0.04599432274699211,0.0503174364566803,0.01718510314822197,0.01021209079772234,0.014724653214216232,-0.009712658822536469,-0.09559711068868637,-0.03537614643573761,0.03641213849186897,0.044450413435697556,-0.04188251122832298,-0.011709102429449558,-0.00415386725217104,-0.027853267267346382,0.06421761959791183,-0.02480657771229744,-0.0806320384144783,0.06836529076099396,0.013005893677473068,-0.018559658899903297,-0.0024560054298490286,0.01807359606027603,0.09325054287910461,0.028918711468577385,0.06992023438215256,-0.08170546591281891,-0.026899494230747223,-0.02450599893927574,0.0422656424343586,0.09773527830839157,0.07804480940103531,0.046469513326883316,0.008213278837502003,-0.021333668380975723,0.03185151144862175,0.06825891137123108,-0.11037246137857437,-0.12419368326663971,0.05576304346323013,-0.0024794440250843763,-0.03401891514658928,0.02073485217988491,-0.0337555967271328,-0.04358541965484619,0.012953214347362518,0.09083133190870285,-0.08631753921508789,0.06195606291294098,0.058942168951034546,-0.029375780373811722,0.011516503989696503,-0.007531076669692993,-0.0014878952642902732,-0.009445038624107838,0.015234185382723808,-0.07742766290903091,0.004044252913445234,0.02157709375023842,-0.034514810889959335,-0.03969581052660942,0.03687545657157898,0.012575732544064522,0.02175127901136875,-0.059165362268686295,-0.0024104153271764517,0.10708992183208466,0.04850078746676445,0.0300979632884264,-0.044371411204338074,0.00872559379786253,0.015455104410648346,0.0365113839507103,-0.013224842958152294,1.0026813998248506e-32,0.03653475269675255,-0.0267704539000988,0.03718297556042671,0.007218323182314634,0.01888546533882618,-0.01685366965830326,0.020731326192617416,0.08751648664474487,-0.05193737521767616,-0.014888981357216835,0.009044667705893517,0.0752270296216011,-0.030469121411442757,0.024723034352064133,-0.017963318154215813,-0.04406377673149109,-0.05550171434879303,0.044120606034994125,-0.015246228314936161,0.00032945870771072805,0.05471044033765793,0.009240162558853626,-0.003934834618121386,-0.03154735267162323,-0.01731543242931366,0.021090662106871605,0.06227341666817665,-0.013300474733114243,-0.08187927305698395,0.034869879484176636,-0.05854259431362152,-0.07362452149391174,0.017638426274061203,0.023019330576062202,0.016039539128541946,-0.017575126141309738,0.07219292223453522,0.01037838589400053,-0.01227116584777832,-0.04106535762548447,0.023818576708436012,-0.009313528425991535,-0.012101760134100914,-0.059319332242012024,-0.05622546374797821,-0.053030189126729965,-0.04826877638697624,0.00187813735101372,0.04120522364974022,0.032117631286382675,0.04679064452648163,0.05008413642644882,0.004230218008160591,-0.023339029401540756,0.056453507393598557,0.0032452093437314034,0.015338240191340446,0.09122084826231003,0.0783076211810112,-0.016147557646036148,-0.0767706111073494,0.06785614788532257,-0.022127125412225723,0.0330079086124897,0.037271611392498016,0.004982593934983015,0.00396264111623168,-0.022280288860201836,0.06875807046890259,-0.06451892107725143,-0.044080667197704315,0.028321299701929092,-0.0006676831981167197,-0.021320221945643425,0.10435234010219574,-0.07529271394014359,-0.035884514451026917,-0.05851992592215538,-0.04445714130997658,-0.047493111342191696,0.01808302104473114,-0.04277963936328888,-0.00297847599722445,0.020690714940428734,0.010976387187838554,0.031714484095573425,0.040775883942842484,-0.09530244022607803,-0.0024344229605048895,-0.016624923795461655,-0.0363621823489666,-0.024272968992590904,-0.0638379380106926,-0.04112337902188301,0.023243946954607964,-1.0162102377768612e-32,0.04665296524763107,-0.005620748270303011,-0.13100674748420715,0.08807486295700073,-0.022683516144752502,-0.02395617589354515,0.03458375483751297,0.05039701238274574,-0.04605291783809662,-0.04823283106088638,0.0014762462815269828,0.03833198547363281,0.0224771648645401,0.006733843591064215,0.06390521675348282,0.04047888517379761,-0.10256660729646683,-0.0752503052353859,0.04453341290354729,0.06877133250236511,-0.0011718733003363013,0.08289550244808197,-0.06480425596237183,0.0389815978705883,-0.04125044494867325,0.04830658808350563,-0.07340739667415619,0.10681163519620895,0.06511939316987991,-0.055839940905570984,-0.011140456423163414,0.04576098546385765,-0.08455919474363327,-0.0424690768122673,-0.06522893160581589,-0.05324292555451393,0.01144514512270689,-0.008010335266590118,0.0035195576492697,0.04929853975772858,0.025862039998173714,-0.05675237998366356,-0.06627876311540604,0.0007093140739016235,-0.04740225151181221,0.012581253424286842,0.05959414318203926,0.03717482462525368,0.013750113546848297,-0.029930179938673973,0.008463950827717781,-0.0205153226852417,-0.10840669274330139,0.07836519926786423,-0.03086814284324646,-0.0016013974091038108,0.06371548026800156,-0.09865804016590118,-0.07782545685768127,0.05385558307170868,-0.0006503646145574749,0.023995978757739067,0.06653045117855072,-0.0819309800863266,0.08787674456834793,-0.03232994303107262,-0.020882463082671165,-0.015531672164797783,-0.0027194612193852663,-0.060629427433013916,-0.024543877691030502,-0.053350258618593216,0.03696107119321823,-0.03914106637239456,0.05141150951385498,0.0034836167469620705,-0.006153784226626158,-0.09768912196159363,0.01659569889307022,-0.014102214947342873,-0.05646759271621704,-0.018229031935334206,0.04825567826628685,0.01897144317626953,0.09175515174865723,-0.02386467345058918,0.0313706174492836,0.0992761105298996,-0.012919249944388866,-0.021119246259331703,-0.010199472308158875,0.05565492436289787,-0.07193243503570557,0.04628363996744156,-0.013375037349760532,-6.126602869471753e-8,-0.08120128512382507,0.04308287054300308,-0.04077048972249031,0.05242808535695076,-0.017847534269094467,0.003772295080125332,0.03413182869553566,0.12739728391170502,0.004747927654534578,-0.06555549055337906,0.042695701122283936,0.07422244548797607,-0.0604698620736599,0.01825551874935627,0.055365901440382004,0.04086323454976082,0.01460951380431652,0.047733791172504425,-0.04766838625073433,-0.01780565083026886,0.01907096616923809,-0.04896598681807518,-0.02700882777571678,-0.03054339811205864,-0.014971066266298294,-0.03416687995195389,0.02443118207156658,0.06274713575839996,0.015198864042758942,-0.0002489279140718281,-0.04510447382926941,0.0618613064289093,-0.05125566944479942,-0.00521731935441494,0.07398135215044022,0.09557748585939407,0.05890202522277832,-0.038925476372241974,0.04920829087495804,0.08483434468507767,0.0774533599615097,0.04882298409938812,-0.13528773188591003,-0.00036108162021264434,0.029201095923781395,0.04063715040683746,-0.04272717982530594,-0.067324697971344,0.05154930427670479,0.05323639139533043,-0.10033044964075089,-0.0026136860251426697,-0.06114301458001137,0.038750309497117996,-0.043948620557785034,0.023412717506289482,0.03391681984066963,-0.09438427537679672,-0.013027219101786613,0.08078431338071823,0.05412700027227402,-0.01244394201785326,0.06371435523033142,0.005405707750469446]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>[summary0.07459140568971634,-0.04399363696575165,0.009493867866694927,0.02547384239733219,0.06932179629802704,-0.007536809425801039,0.08027100563049316,0.007233878131955862,-0.07480641454458237,0.0025095201563090086,0.010290723294019699,0.07750000804662704,-0.036116763949394226,0.00832766480743885,0.02931866981089115,0.03598008677363396,0.0272238627076149,-0.1048184186220169,-0.02308756485581398,0.024795398116111755,0.013782665133476257,0.020406315103173256,0.010608009062707424,-0.000995631911791861,-0.018737860023975372,0.044051311910152435,0.01809786818921566,-0.17600105702877045,-0.016276374459266663,0.0594552680850029,0.03966787829995155,-0.040495615452528,0.05969705432653427,0.04100668057799339,-0.04240217059850693,0.05698563903570175,0.02676762267947197,0.03144058585166931,-0.05112902820110321,0.017340004444122314,0.020167572423815727,0.04034119471907616,-0.059214282780885696,-0.08174728602170944,-0.03932853415608406,-0.13129308819770813,-0.005795750766992569,-0.11669299751520157,0.016903115436434746,0.005350644700229168,-0.036449648439884186,-0.01816623844206333,0.07921068370342255,0.003422764129936695,-0.020575521513819695,0.058947641402482986,-0.00767391175031662,0.08071301132440567,-0.008195952512323856,0.07243737578392029,-0.08523273468017578,-0.030774572864174843,0.001745138200931251,-0.10726328939199448,0.04435501992702484,0.08007928729057312,0.08393874764442444,0.010593230836093426,-0.015723146498203278,0.024355445057153702,0.03666283190250397,0.010213888250291348,0.025618767365813255,-0.017869748175144196,0.03137589991092682,-0.019215203821659088,-0.06120220571756363,-0.019701845943927765,0.10789471119642258,-0.0934130996465683,-0.04536743462085724,0.01273997500538826,-0.10229448229074478,-0.07867416739463806,0.029002828523516655,-0.015330435708165169,-0.021803895011544228,0.009053303860127926,-0.014773625880479813,-0.02372046932578087,0.015410782769322395,-0.010834087617695332,-0.09306301176548004,-0.052429333329200745,0.04649189114570618,-0.07034384459257126,0.11425468325614929,-0.003319780807942152,-0.041670359671115875,-0.05615558475255966,-0.03527223691344261,0.10309033840894699,0.06378267705440521,0.03868015855550766,-0.03234630450606346,0.042461197823286057,0.05868852138519287,-0.007295587100088596,-0.05395372584462166,-0.004737584386020899,-0.0609157495200634,0.024208690971136093,0.07584479451179504,-0.002147630089893937,0.03773428499698639,-0.06090541183948517,-0.12339921295642853,-0.07903692126274109,-0.04652228206396103,-0.047100141644477844,0.04196273908019066,-0.004814604297280312,0.006123455706983805,0.0567636601626873,0.05292699858546257,0.039825376123189926,-0.1005186215043068,2.5507692930256e-33,0.0026602400466799736,-0.014316392131149769,-0.07570024579763412,0.05127689614892006,-0.014932462014257908,0.03681743144989014,0.04206416383385658,0.01278188731521368,0.08602829277515411,0.013412805274128914,0.004404681269079447,-0.09025078266859055,0.050810307264328,0.015039291232824326,-0.06082998588681221,-0.02296430990099907,0.03862236067652702,-0.03534051403403282,0.004474210552871227,0.06207694485783577,-0.02436605468392372,0.001856986666098237,-0.07854974269866943,0.03399404510855675,-0.10388889163732529,0.009039290249347687,-0.007294348441064358,0.0736326277256012,0.024401525035500526,0.04334666207432747,0.052406132221221924,-0.01168495137244463,-0.14248813688755035,0.02564247138798237,-0.05182601138949394,-0.02016608603298664,0.03373769670724869,0.0412910096347332,0.020291727036237717,-0.0635184571146965,-0.05893813073635101,0.01361008919775486,0.007021849974989891,0.042819052934646606,-0.02414429746568203,0.07414299994707108,0.06315026432275772,-0.06256907433271408,-0.03570788726210594,-0.014807925559580326,0.025114301592111588,-0.0065802112221717834,0.003598087001591921,-0.06035885959863663,-0.02831011265516281,0.04927346110343933,0.01380492839962244,-0.036906275898218155,-0.04010811075568199,0.09211521595716476,0.1135915145277977,-0.026858024299144745,-0.05661778151988983,0.028187083080410957,-0.028117898851633072,0.037332069128751755,0.07247045636177063,0.06522390991449356,-0.0143169816583395,0.03793087601661682,0.07652518898248672,-0.01896503195166588,-0.02695869468152523,0.024658210575580597,0.07150197774171829,-0.0587569959461689,0.038147661834955215,-0.10210389643907547,-0.05735000595450401,-0.04727257788181305,-0.029810914769768715,-0.07256493717432022,0.03168348968029022,0.02493860572576523,-0.058575186878442764,-0.06942219287157059,-0.0477314367890358,0.10114060342311859,-0.1145133301615715,0.03713619336485863,0.026791103184223175,-0.004317635670304298,0.019255297258496284,0.08501052111387253,0.03733247146010399,-4.881331025259753e-33,0.01980195753276348,0.03540078178048134,0.012756800279021263,-0.09854022413492203,-0.050012048333883286,0.041725460439920425,0.03545377030968666,0.02325555309653282,-0.0002519113477319479,-0.029363149777054787,-0.02443843148648739,-0.02073141559958458,-0.02122850902378559,-0.02043175883591175,-0.015286268666386604,0.01371963694691658,-0.008552678860723972,0.07867570221424103,0.07787328213453293,0.005523102357983589,0.027772989124059677,-0.030111238360404968,-0.03786662593483925,-0.005087751429527998,0.005073714070022106,0.005952497012913227,-0.025130804628133774,0.020368877798318863,-0.05295553058385849,0.04725082963705063,0.03342621773481369,0.008648485876619816,0.07206545025110245,-0.010116958990693092,-0.02611006610095501,0.0016963580856099725,-0.12509095668792725,-0.041952524334192276,-0.10521429032087326,-0.01809699460864067,-0.014475706033408642,-0.04544403403997421,0.0834507867693901,0.014312624000012875,-0.009623514488339424,0.025170838460326195,-0.010092793963849545,0.016579926013946533,-0.07655782252550125,0.07884599268436432,0.0701896920800209,0.031785592436790466,0.07741570472717285,-0.051625970751047134,-0.09341736882925034,0.03326738625764847,-0.051006074994802475,-0.011509322561323643,0.0428006649017334,-0.021116333082318306,0.05688844993710518,0.006312720011919737,-0.048160601407289505,0.010945831425487995,-0.04775554686784744,-0.03014681674540043,0.049462538212537766,-0.00031822884920984507,0.05320311710238457,0.016807133331894875,0.04666650667786598,0.03033570386469364,-0.04754628986120224,0.06681416183710098,-0.045037638396024704,-0.036073364317417145,-0.05904775857925415,0.051379863172769547,-0.018847549334168434,-0.06394612044095993,0.00230729510076344,0.021194536238908768,-0.002548307878896594,0.04142607003450394,-0.1452922523021698,0.0032699587754905224,0.04944748431444168,-0.058300700038671494,-0.007470255251973867,-0.028319524601101875,0.01270403154194355,0.028292648494243622,-0.11760968714952469,0.06432235240936279,-0.002733251778408885,-3.8421212877892685e-8,0.04852527007460594,0.014425174333155155,0.04416472092270851,-0.005156221799552441,0.019639931619167328,0.024109240621328354,-0.0019345898181200027,0.06125693768262863,-0.021681977435946465,0.007821149192750454,-0.05714309215545654,-0.0018091789679601789,-0.027982404455542564,-0.07891734689474106,0.021832682192325592,-0.07941294461488724,0.003944438882172108,0.021416477859020233,-0.003290091175585985,-0.008432977832853794,0.04929070174694061,-0.0468762069940567,-0.005811365321278572,-0.03560729697346687,-0.03977213799953461,-0.06672830879688263,0.0025222646072506905,-0.041288748383522034,-0.05136365815997124,-0.04168880358338356,0.10465890914201736,0.0008506066515110433,0.0014335991581901908,-0.0008890560711733997,0.010082051157951355,-0.037270914763212204,0.018628934398293495,-0.03336012735962868,-0.0300067700445652,0.0523429811000824,-0.060446999967098236,0.012174070812761784,0.06004902347922325,-0.01640998385846615,-0.00712950062006712,0.0037197379861027002,-0.05373059958219528,-0.09015827625989914,0.14175042510032654,0.03515839949250221,0.05407901480793953,0.028623441234230995,0.03464437276124954,-0.06084984168410301,-0.006482816766947508,0.0254029780626297,-0.042437467724084854,0.04007820412516594,-0.060530513525009155,0.04436290264129639,0.07808824628591537,0.09748309850692749,-0.05496140569448471,-0.00045077266986481845]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>[0.04199979826807976,-0.01682301238179207,0.03257901966571808,0.050000134855508804,0.012687240727245808,0.02664201334118843,0.047926612198352814,0.023782406002283096,-0.05115845426917076,0.005681084003299475,0.009550634771585464,0.04887887090444565,-0.017743535339832306,0.08157909661531448,0.03556184098124504,0.059909969568252563,0.06259191781282425,0.0028343473095446825,-0.04470386728644371,0.04607988893985748,-0.017361892387270927,0.009841710329055786,0.030243640765547752,0.025770289823412895,-0.08138974010944366,0.05313200131058693,0.013454822823405266,-0.13718010485172272,-0.09762075543403625,0.0512353889644146,0.05622950941324234,-0.011792272329330444,0.06043342500925064,0.05597600340843201,-0.027147572487592697,0.07398045063018799,-0.04008066654205322,0.048537369817495346,-0.038795966655015945,-0.012787006795406342,-0.009400567039847374,0.030877549201250076,-0.06282996386289597,-0.07415446639060974,-0.0170640517026186,-0.13542678952217102,0.01000860147178173,-0.09039566665887833,-0.006852397229522467,-0.01416865922510624,-0.02003927156329155,-0.007522843778133392,0.05883470177650452,0.01683897152543068,-0.0005259496974758804,0.0691593810915947,-0.003416825318709016,0.04325870797038078,-0.005326145328581333,0.04626961797475815,-0.0949285700917244,0.022739022970199585,-0.009496256709098816,-0.1586163491010666,0.05885534733533859,0.06084056198596954,0.05459442734718323,-0.027192041277885437,0.033056873828172684,-0.04752041772007942,-0.04397017881274223,0.03458554670214653,0.0343838632106781,-0.0025384495966136456,0.027265939861536026,0.030350906774401665,-0.029902763664722443,-0.0028187287971377373,0.07587487995624542,-0.08541379868984222,0.0059251743368804455,0.06326436251401901,-0.08503750711679459,-0.07779958844184875,0.05097121745347977,-0.021576307713985443,0.028771353885531425,0.02286563254892826,-0.013819974847137928,-0.04005897417664528,0.055137477815151215,-0.023651331663131714,-0.07651237398386002,-0.04419563338160515,0.13729844987392426,-0.06334075331687927,0.0968041643500328,0.022144386544823647,-0.039838746190071106,-0.06630147993564606,-0.007788613438606262,0.06121494248509407,0.02391025982797146,0.015075678937137127,-0.03282272443175316,0.044567208737134933,0.022355757653713226,-0.019111210480332375,-0.04575822502374649,-0.05089764669537544,-0.07436080276966095,-0.010623442009091377,0.05882072448730469,-0.01315570343285799,-0.01614597626030445,-0.03285918012261391,-0.05666425824165344,-0.04972117766737938,-0.02639087848365307,-0.039389681071043015,0.05198191478848457,-0.025633085519075394,0.08397037535905838,0.02779691107571125,0.04724135622382164,0.023292632773518562,-0.08119619637727737,8.797029440833491e-33,-0.03837834298610687,0.03162718564271927,-0.07975959032773972,-0.011762771755456924,-0.044736988842487335,0.04975870996713638,0.056364793330430984,0.022641636431217194,0.05647306889295578,-0.014653576537966728,0.015822159126400948,-0.04095717519521713,0.08504787087440491,0.02912670001387596,-0.0195663720369339,0.003931893035769463,-0.0018850486958399415,-0.010148303583264351,-0.024462511762976646,0.09762454032897949,-0.035956691950559616,0.0630096048116684,-0.02840443141758442,0.03260655701160431,-0.05303645506501198,-0.02658124640583992,0.009244012646377087,0.03896833211183548,-0.0038408429827541113,0.011091720312833786,0.03578909859061241,-0.02695818804204464,-0.09257593750953674,-0.0037537976168096066,-0.06438282877206802,-0.04419593885540962,0.04579666256904602,0.001688522519543767,-0.021033944562077522,-0.06785060465335846,-0.031870581209659576,0.0020237104035913944,-0.033808059990406036,0.08573657274246216,-0.00949388649314642,0.06476454436779022,0.03758411109447479,-0.018257027491927147,-0.03007536195218563,0.022264406085014343,0.049254514276981354,0.0128695173189044,-0.07460702210664749,-0.14536255598068237,-0.06215813755989075,0.043484173715114594,0.03541459143161774,-0.03747271001338959,-0.0002865921414922923,0.08220063894987106,0.0780380442738533,-0.028101269155740738,-0.06012478470802307,0.03027285635471344,-0.031050534918904305,0.008143875747919083,0.06869126856327057,0.02828097715973854,0.019404567778110504,0.009003221988677979,0.011029863730072975,-0.03990757092833519,0.09844827651977539,0.09887844324111938,0.045030828565359116,-0.04639400169253349,0.04487818107008934,-0.061087775975465775,-0.07476513087749481,-0.07291877269744873,-0.023449117317795753,-0.05335462465882301,0.043137501925230026,-0.0019896815065294504,-0.0675245001912117,-0.031202521175146103,-0.09116147458553314,0.08702316880226135,-0.09915554523468018,-0.035132624208927155,0.06039038300514221,-0.012937711551785469,-0.010442067869007587,0.1262413114309311,0.03262512385845184,-7.989036501064498e-33,0.06081204116344452,0.021744826808571815,-0.009593883529305458,-0.13206510245800018,-0.026792412623763084,0.04117802157998085,0.02635789103806019,-0.04744815453886986,0.031700652092695236,-0.10164511948823929,-0.04132525250315666,-0.0017599458806216717,-0.019587308168411255,-0.012821950018405914,-0.039385270327329636,0.040853749960660934,-0.02322760783135891,0.06273780763149261,0.0048382640816271305,0.03564796969294548,0.019180072471499443,0.05126870423555374,-0.04176655039191246,-0.018677206709980965,0.06715801358222961,0.025190886110067368,-0.03437618538737297,0.05161343142390251,0.04872404411435127,0.05924582481384277,0.048530057072639465,0.05231572315096855,0.04056892916560173,-0.028941655531525612,-0.010349913500249386,-0.004092592280358076,-0.04879887402057648,-0.056601691991090775,-0.11338310688734055,-0.007204810623079538,0.01238926313817501,0.016560455784201622,0.07112521678209305,0.024530835449695587,0.013772204518318176,0.12171462923288345,-0.024470068514347076,-0.024785125628113747,-0.056625962257385254,0.10693618655204773,0.05873417854309082,0.0028362805023789406,0.03480609133839607,-0.05197567865252495,-0.03310994803905487,0.030346181243658066,-0.04574596881866455,-0.048641446977853775,-0.02525821328163147,-0.07152964174747467,0.038677748292684555,-0.013249066658318043,0.01474758516997099,0.030177714303135872,-0.025663945823907852,0.013643897138535976,0.018138187006115913,-0.0197981558740139,0.07472532987594604,-0.020256197080016136,-0.014606952667236328,0.005036862567067146,0.005130034405738115,-0.017326608300209045,0.040368396788835526,0.018261970952153206,-0.052796557545661926,0.047545820474624634,-0.04190578684210777,-0.03161892294883728,0.002250197809189558,0.010005303658545017,0.023101484403014183,-0.0006794763030484319,-0.11093278229236603,-0.006944555789232254,0.006063944194465876,-0.055398013442754745,0.017270565032958984,-0.022290078923106194,-0.017096826806664467,0.04098721593618393,-0.1268056184053421,0.006956424564123154,0.009653765708208084,-6.169432253955165e-8,0.06945820897817612,-0.05264206603169441,0.018784964457154274,-0.0344930961728096,-0.0021150116808712482,-0.0185861773788929,-0.03468076139688492,0.11411607265472412,-0.03531566262245178,0.07253412902355194,-0.029719091951847076,0.014490211382508278,-0.06519311666488647,-0.07670686393976212,0.008845246396958828,-0.07751346379518509,-0.0019552260637283325,0.036375731229782104,-0.02353476919233799,0.025279328227043152,0.006874028127640486,-0.012661985121667385,-0.0135008180513978,-0.015973854809999466,-0.02914472483098507,-0.055144764482975006,0.046673163771629333,-0.004516617860645056,-0.04304014518857002,-0.06605894863605499,0.10450497269630432,-0.034582581371068954,0.053905073553323746,0.009035224094986916,0.017692387104034424,-0.11112909764051437,0.06677822768688202,-0.020457860082387924,-0.023511625826358795,0.14538083970546722,0.0030021967831999063,0.0062972987070679665,0.07279672473669052,0.004087503533810377,0.032760296016931534,-0.04380064085125923,-0.08563249558210373,-0.0912184864282608,0.12184514850378036,0.007806412875652313,0.04818987846374512,0.02308233082294464,-0.016948889940977097,-0.08151108026504517,-0.020747505128383636,0.04984244331717491,-0.02308920957148075,0.009684446267783642,-0.0545465461909771,-0.01164942979812622,0.07416947931051254,0.10190920531749725,-0.018531838431954384,0.02400047890841961]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -3716,6 +3700,54 @@
   </si>
   <si>
     <t>Embedding</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[0.07459140568971634,-0.04399363696575165,0.009493867866694927,0.02547384239733219,0.06932179629802704,-0.007536809425801039,0.08027100563049316,0.007233878131955862,-0.07480641454458237,0.0025095201563090086,0.010290723294019699,0.07750000804662704,-0.036116763949394226,0.00832766480743885,0.02931866981089115,0.03598008677363396,0.0272238627076149,-0.1048184186220169,-0.02308756485581398,0.024795398116111755,0.013782665133476257,0.020406315103173256,0.010608009062707424,-0.000995631911791861,-0.018737860023975372,0.044051311910152435,0.01809786818921566,-0.17600105702877045,-0.016276374459266663,0.0594552680850029,0.03966787829995155,-0.040495615452528,0.05969705432653427,0.04100668057799339,-0.04240217059850693,0.05698563903570175,0.02676762267947197,0.03144058585166931,-0.05112902820110321,0.017340004444122314,0.020167572423815727,0.04034119471907616,-0.059214282780885696,-0.08174728602170944,-0.03932853415608406,-0.13129308819770813,-0.005795750766992569,-0.11669299751520157,0.016903115436434746,0.005350644700229168,-0.036449648439884186,-0.01816623844206333,0.07921068370342255,0.003422764129936695,-0.020575521513819695,0.058947641402482986,-0.00767391175031662,0.08071301132440567,-0.008195952512323856,0.07243737578392029,-0.08523273468017578,-0.030774572864174843,0.001745138200931251,-0.10726328939199448,0.04435501992702484,0.08007928729057312,0.08393874764442444,0.010593230836093426,-0.015723146498203278,0.024355445057153702,0.03666283190250397,0.010213888250291348,0.025618767365813255,-0.017869748175144196,0.03137589991092682,-0.019215203821659088,-0.06120220571756363,-0.019701845943927765,0.10789471119642258,-0.0934130996465683,-0.04536743462085724,0.01273997500538826,-0.10229448229074478,-0.07867416739463806,0.029002828523516655,-0.015330435708165169,-0.021803895011544228,0.009053303860127926,-0.014773625880479813,-0.02372046932578087,0.015410782769322395,-0.010834087617695332,-0.09306301176548004,-0.052429333329200745,0.04649189114570618,-0.07034384459257126,0.11425468325614929,-0.003319780807942152,-0.041670359671115875,-0.05615558475255966,-0.03527223691344261,0.10309033840894699,0.06378267705440521,0.03868015855550766,-0.03234630450606346,0.042461197823286057,0.05868852138519287,-0.007295587100088596,-0.05395372584462166,-0.004737584386020899,-0.0609157495200634,0.024208690971136093,0.07584479451179504,-0.002147630089893937,0.03773428499698639,-0.06090541183948517,-0.12339921295642853,-0.07903692126274109,-0.04652228206396103,-0.047100141644477844,0.04196273908019066,-0.004814604297280312,0.006123455706983805,0.0567636601626873,0.05292699858546257,0.039825376123189926,-0.1005186215043068,2.5507692930256e-33,0.0026602400466799736,-0.014316392131149769,-0.07570024579763412,0.05127689614892006,-0.014932462014257908,0.03681743144989014,0.04206416383385658,0.01278188731521368,0.08602829277515411,0.013412805274128914,0.004404681269079447,-0.09025078266859055,0.050810307264328,0.015039291232824326,-0.06082998588681221,-0.02296430990099907,0.03862236067652702,-0.03534051403403282,0.004474210552871227,0.06207694485783577,-0.02436605468392372,0.001856986666098237,-0.07854974269866943,0.03399404510855675,-0.10388889163732529,0.009039290249347687,-0.007294348441064358,0.0736326277256012,0.024401525035500526,0.04334666207432747,0.052406132221221924,-0.01168495137244463,-0.14248813688755035,0.02564247138798237,-0.05182601138949394,-0.02016608603298664,0.03373769670724869,0.0412910096347332,0.020291727036237717,-0.0635184571146965,-0.05893813073635101,0.01361008919775486,0.007021849974989891,0.042819052934646606,-0.02414429746568203,0.07414299994707108,0.06315026432275772,-0.06256907433271408,-0.03570788726210594,-0.014807925559580326,0.025114301592111588,-0.0065802112221717834,0.003598087001591921,-0.06035885959863663,-0.02831011265516281,0.04927346110343933,0.01380492839962244,-0.036906275898218155,-0.04010811075568199,0.09211521595716476,0.1135915145277977,-0.026858024299144745,-0.05661778151988983,0.028187083080410957,-0.028117898851633072,0.037332069128751755,0.07247045636177063,0.06522390991449356,-0.0143169816583395,0.03793087601661682,0.07652518898248672,-0.01896503195166588,-0.02695869468152523,0.024658210575580597,0.07150197774171829,-0.0587569959461689,0.038147661834955215,-0.10210389643907547,-0.05735000595450401,-0.04727257788181305,-0.029810914769768715,-0.07256493717432022,0.03168348968029022,0.02493860572576523,-0.058575186878442764,-0.06942219287157059,-0.0477314367890358,0.10114060342311859,-0.1145133301615715,0.03713619336485863,0.026791103184223175,-0.004317635670304298,0.019255297258496284,0.08501052111387253,0.03733247146010399,-4.881331025259753e-33,0.01980195753276348,0.03540078178048134,0.012756800279021263,-0.09854022413492203,-0.050012048333883286,0.041725460439920425,0.03545377030968666,0.02325555309653282,-0.0002519113477319479,-0.029363149777054787,-0.02443843148648739,-0.02073141559958458,-0.02122850902378559,-0.02043175883591175,-0.015286268666386604,0.01371963694691658,-0.008552678860723972,0.07867570221424103,0.07787328213453293,0.005523102357983589,0.027772989124059677,-0.030111238360404968,-0.03786662593483925,-0.005087751429527998,0.005073714070022106,0.005952497012913227,-0.025130804628133774,0.020368877798318863,-0.05295553058385849,0.04725082963705063,0.03342621773481369,0.008648485876619816,0.07206545025110245,-0.010116958990693092,-0.02611006610095501,0.0016963580856099725,-0.12509095668792725,-0.041952524334192276,-0.10521429032087326,-0.01809699460864067,-0.014475706033408642,-0.04544403403997421,0.0834507867693901,0.014312624000012875,-0.009623514488339424,0.025170838460326195,-0.010092793963849545,0.016579926013946533,-0.07655782252550125,0.07884599268436432,0.0701896920800209,0.031785592436790466,0.07741570472717285,-0.051625970751047134,-0.09341736882925034,0.03326738625764847,-0.051006074994802475,-0.011509322561323643,0.0428006649017334,-0.021116333082318306,0.05688844993710518,0.006312720011919737,-0.048160601407289505,0.010945831425487995,-0.04775554686784744,-0.03014681674540043,0.049462538212537766,-0.00031822884920984507,0.05320311710238457,0.016807133331894875,0.04666650667786598,0.03033570386469364,-0.04754628986120224,0.06681416183710098,-0.045037638396024704,-0.036073364317417145,-0.05904775857925415,0.051379863172769547,-0.018847549334168434,-0.06394612044095993,0.00230729510076344,0.021194536238908768,-0.002548307878896594,0.04142607003450394,-0.1452922523021698,0.0032699587754905224,0.04944748431444168,-0.058300700038671494,-0.007470255251973867,-0.028319524601101875,0.01270403154194355,0.028292648494243622,-0.11760968714952469,0.06432235240936279,-0.002733251778408885,-3.8421212877892685e-8,0.04852527007460594,0.014425174333155155,0.04416472092270851,-0.005156221799552441,0.019639931619167328,0.024109240621328354,-0.0019345898181200027,0.06125693768262863,-0.021681977435946465,0.007821149192750454,-0.05714309215545654,-0.0018091789679601789,-0.027982404455542564,-0.07891734689474106,0.021832682192325592,-0.07941294461488724,0.003944438882172108,0.021416477859020233,-0.003290091175585985,-0.008432977832853794,0.04929070174694061,-0.0468762069940567,-0.005811365321278572,-0.03560729697346687,-0.03977213799953461,-0.06672830879688263,0.0025222646072506905,-0.041288748383522034,-0.05136365815997124,-0.04168880358338356,0.10465890914201736,0.0008506066515110433,0.0014335991581901908,-0.0008890560711733997,0.010082051157951355,-0.037270914763212204,0.018628934398293495,-0.03336012735962868,-0.0300067700445652,0.0523429811000824,-0.060446999967098236,0.012174070812761784,0.06004902347922325,-0.01640998385846615,-0.00712950062006712,0.0037197379861027002,-0.05373059958219528,-0.09015827625989914,0.14175042510032654,0.03515839949250221,0.05407901480793953,0.028623441234230995,0.03464437276124954,-0.06084984168410301,-0.006482816766947508,0.0254029780626297,-0.042437467724084854,0.04007820412516594,-0.060530513525009155,0.04436290264129639,0.07808824628591537,0.09748309850692749,-0.05496140569448471,-0.00045077266986481845]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[-0.08861415833234787,-0.0416453517973423,-0.015285965986549854,-0.031236819922924042,-0.033545151352882385,-0.07572811096906662,-0.10687108337879181,0.03258390724658966,-0.03055522032082081,-0.061724480241537094,-0.0868893712759018,0.01353105716407299,-0.0398903526365757,-0.020236173644661903,0.0008984606829471886,-0.0006998720346018672,-0.01256787683814764,0.032651323825120926,-0.09016240388154984,-0.08588181436061859,0.0677943155169487,0.07395553588867188,-0.047948818653821945,0.028694458305835724,-0.05736779421567917,0.004636651836335659,0.00591965252533555,-0.006066696252673864,-0.02472926862537861,0.006809897720813751,-0.03353552147746086,-0.0588238462805748,-0.045347586274147034,0.04337560757994652,-0.05396323278546333,0.05274508520960808,0.10195180773735046,0.0046644131653010845,-0.005802451632916927,-0.01412081066519022,-0.003974903840571642,-0.08620896935462952,-0.042115408927202225,-0.03712967410683632,0.05351204052567482,-0.026932811364531517,-0.07879295200109482,-0.17889705300331116,-0.06903326511383057,0.03425119072198868,-0.03597957640886307,-0.07212844491004944,-0.06990452855825424,0.04909346252679825,-0.04596942663192749,0.05464037507772446,0.055095043033361435,0.0012528729857876897,-0.042321473360061646,-0.051551371812820435,-0.05317028611898422,-0.061922501772642136,0.007018471602350473,0.0801953375339508,-0.02182837948203087,-0.016811922192573547,-0.0007797287544235587,0.004563171416521072,0.1129416674375534,-0.07983756810426712,-0.036265794187784195,0.012442623265087605,-0.021289536729454994,0.015719473361968994,-0.008191955275833607,0.0005369919235818088,0.0716916024684906,0.05802719667553902,0.010085883550345898,-0.013016822747886181,-0.03149092197418213,0.0008126820903271437,0.03391913324594498,0.0351218655705452,-0.0012321402318775654,0.09957783669233322,-0.03473298251628876,0.01759064383804798,-0.006292752921581268,-0.010538148693740368,-0.07222137600183487,-0.06961370259523392,0.06497926265001297,0.024056436493992805,-0.04321344196796417,0.019089121371507645,-0.022440992295742035,-0.0606020987033844,0.05867739021778107,0.02050013095140457,-0.10296349972486496,0.0010142280953004956,0.05314956605434418,-0.04463727027177811,-0.0054864464327692986,-0.005001158453524113,-0.06561466306447983,0.0008229342056438327,-0.015629954636096954,-0.10465411841869354,-0.010522997938096523,-0.07345084846019745,-0.03836608678102493,-0.03453730046749115,0.05854957550764084,0.011030161753296852,-0.06866592168807983,-0.060371801257133484,-0.043643802404403687,0.10413865000009537,-0.07586723566055298,-0.00677602831274271,0.010421248152852058,-0.004999800585210323,0.018629400059580803,-0.03386705741286278,-0.07112549245357513,-2.5207098820941586e-33,0.013758925721049309,-0.07242990285158157,0.04763162136077881,-0.02728687971830368,0.11022943258285522,-0.0038848603144288063,0.07208802551031113,0.014302851632237434,-0.07304053008556366,0.007392518687993288,0.02348690666258335,0.05164490267634392,-0.012890974059700966,0.06742703914642334,-0.026047799736261368,-0.008445088751614094,-0.03674953430891037,0.05177466943860054,-0.023166967555880547,0.019007643684744835,0.014282935298979282,0.08918444812297821,0.0029961951076984406,0.004966838285326958,0.06445526331663132,-0.032637789845466614,0.05134573578834534,0.03599756956100464,-0.07789025455713272,0.037986088544130325,-0.00034893411793746054,-0.02653220109641552,0.032696306705474854,-0.05813044309616089,0.001452227937988937,0.0035141934640705585,0.04209515452384949,0.033978287130594254,0.019025545567274094,-0.02875804528594017,0.029954198747873306,-0.0010368252405896783,0.020446037873625755,-0.025818511843681335,-0.04999670758843422,0.0006745914579369128,-0.052610501646995544,-0.04814746603369713,-0.013064569793641567,-0.01145867072045803,0.04226132109761238,-0.02357134036719799,0.062217872589826584,0.02158433385193348,0.03960482403635979,-0.055696040391922,0.03568805754184723,0.06762305647134781,0.0030761242378503084,0.005637252703309059,-0.0003492495743557811,0.044130146503448486,-0.007610798347741365,0.0826956108212471,-0.020507361739873886,0.0003651201259344816,0.03904897719621658,0.04302101582288742,0.05530036240816116,0.05925678834319115,0.006584573537111282,0.07746513932943344,-0.0499606654047966,0.02054445818066597,0.09567726403474808,-0.009975663386285305,0.03237108513712883,-0.017686204984784126,-0.039641834795475006,0.05650966241955757,-0.05990104377269745,0.023806730285286903,0.021921910345554352,0.008154737763106823,-0.06014057993888855,0.07935377210378647,-0.044360142201185226,-0.003782201325520873,0.006763943005353212,-0.0003828492190223187,-0.09389795362949371,0.000054601892770733684,-0.05495423823595047,0.054075781255960464,0.03652456775307655,-1.7999812348263972e-33,0.090720996260643,0.09758063405752182,-0.07674086838960648,0.10562846809625626,0.004586813505738974,0.017922764644026756,-0.0002830916200764477,-0.06786663085222244,-0.022855618968605995,0.021228056401014328,-0.03355248272418976,0.1072133257985115,0.029428629204630852,0.08279737830162048,0.034095000475645065,-0.07068140804767609,-0.11346441507339478,-0.17287881672382355,0.0354776531457901,-0.0022358535788953304,-0.03799431025981903,0.02483353205025196,-0.02319561317563057,-0.018046550452709198,-0.03456777334213257,-0.01572038233280182,-0.1602235585451126,0.01973070576786995,0.04674682393670082,0.00009814972872845829,-0.026997599750757217,-0.011161626316606998,0.025988390669226646,-0.09159308671951294,-0.10149852931499481,0.06374502927064896,0.02326209470629692,0.03570591285824776,0.11226183921098709,-0.012813873589038849,-0.04926786199212074,-0.043155983090400696,0.025612110272049904,-0.07972483336925507,-0.09115728735923767,0.04140958935022354,0.10224860906600952,0.006081623025238514,-0.034435804933309555,-0.05353683978319168,-0.03457590565085411,0.06834147870540619,-0.02500440925359726,0.05432803928852081,0.009177790023386478,0.021600352600216866,-0.025098955258727074,0.0035928827710449696,-0.09587088227272034,0.017864150926470757,-0.016726769506931305,0.030506322160363197,0.03253728151321411,0.04285847395658493,-0.0837063416838646,0.005900312215089798,-0.025416040793061256,-0.02105499804019928,-0.003458706894889474,-0.020637670531868935,0.009767448529601097,-0.0011290267575532198,-0.022551631554961205,0.06482832133769989,-0.022782811895012856,-0.0642748773097992,-0.04789303243160248,-0.00007090232247719541,0.010205984115600586,0.07964382320642471,-0.014162492007017136,-0.015352866612374783,0.0002947983448393643,0.10473450273275375,0.1088242307305336,-0.038245789706707,0.08964421600103378,-0.019832724705338478,0.004042681772261858,-0.02960776351392269,0.01737804338335991,0.07548071444034576,-0.08385809510946274,-0.00756809301674366,-0.03056159056723118,-3.254081804016096e-8,0.0028776731342077255,0.03218218684196472,0.05953732505440712,0.059806421399116516,-0.023162154480814934,-0.012764208018779755,0.01997974142432213,0.1640552282333374,0.0035036078188568354,0.03133802488446236,0.0019289960619062185,-0.014055952429771423,-0.021145693957805634,0.0153757743537426,0.030150674283504486,0.06827739626169205,0.03570759668946266,0.0390823669731617,0.0035134884528815746,-0.005935993976891041,0.019441552460193634,-0.03830980509519577,0.008445159532129765,-0.012935638427734375,-0.028229134157299995,-0.056522585451602936,0.05233171954751015,0.0075251078233122826,-0.01999911107122898,0.011988567188382149,-0.08123207092285156,0.020788805559277534,-0.019000766798853874,-0.04794834926724434,0.1459568589925766,0.07134490460157394,-0.01870449259877205,-0.0384332649409771,-0.016004623845219612,0.018292609602212906,0.025270944461226463,-0.04467513784766197,0.01622607558965683,0.00005706916272174567,-0.01431744359433651,0.061732739210128784,0.007022933103144169,-0.04232361167669296,-0.029704125598073006,0.06466051936149597,-0.058940988034009933,0.031334418803453445,-0.019404256716370583,0.06287102401256561,-0.006035404745489359,0.04396717622876167,0.05071181803941727,-0.12261836230754852,-0.008913788944482803,0.03406069427728653,0.01285090297460556,0.06872457265853882,0.08229980617761612,-0.041040051728487015]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://blog.dataiku.com/large-language-model-chatgpt</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[-0.09475500136613846,-0.06114489585161209,0.009902226738631725,0.05530209466814995,0.0009779937099665403,-0.021011846140027046,0.04742660000920296,-0.02551255375146866,0.0979108139872551,-0.041475411504507065,-0.02022479847073555,0.018518634140491486,-0.0035198545083403587,-0.03446377068758011,0.05515746772289276,0.03325895965099335,0.05933716520667076,-0.02677459456026554,-0.0499575212597847,-0.06424164026975632,0.0737195536494255,0.0710643082857132,0.06138497218489647,-0.016177373006939888,0.016292549669742584,0.0511348657310009,-0.020079439505934715,-0.04298589378595352,0.0655435174703598,0.028962014243006706,0.0657215267419815,0.01809507980942726,0.04390151798725128,0.06188075989484787,-0.0801788792014122,0.04349253699183464,-0.050756871700286865,-0.010124992579221725,0.032311804592609406,-0.018518930301070213,-0.003956812899559736,-0.05433761700987816,0.04682854562997818,0.014920946210622787,0.12063978612422943,0.012099102139472961,-0.0673440620303154,0.004984698724001646,0.0022427760995924473,0.0388515405356884,-0.11065894365310669,-0.02387826517224312,0.05216545984148979,0.04265027120709419,-0.0009735695202834904,0.08263099938631058,-0.036589108407497406,0.05026255175471306,0.030408237129449844,-0.01824326254427433,0.0028939200565218925,-0.02860090136528015,0.02481100894510746,-0.04114321619272232,0.02275216206908226,-0.026488078758120537,-0.029720338061451912,0.01000506617128849,0.018507737666368484,-0.08976426720619202,0.06643255054950714,0.0551622174680233,0.030388614162802696,0.006562176160514355,-0.017452901229262352,0.06684570014476776,0.03351617231965065,-0.039626434445381165,0.043672505766153336,-0.0030301560182124376,0.001414735452271998,-0.0312271099537611,0.08819752186536789,0.031196553260087967,-0.03671940043568611,0.039136286824941635,0.05874275043606758,0.056306105107069016,-0.009742481634020805,0.03537929430603981,-0.05322205647826195,-0.04683070257306099,0.06618200987577438,-0.01920468360185623,-0.04182466119527817,-0.007253678981214762,-0.023678842931985855,-0.0361788384616375,-0.052494168281555176,0.0828789472579956,-0.013879401609301567,0.0023409733548760414,0.008256743662059307,-0.04785268381237984,-0.032821428030729294,-0.008051167242228985,0.06416122615337372,0.005769032519310713,0.03986865282058716,-0.04343699663877487,-0.018414638936519623,-0.071693554520607,0.031248752027750015,-0.019184106960892677,0.05762254074215889,-0.0038018422201275826,-0.043574489653110504,-0.01085598859935999,0.040392905473709106,0.07335279136896133,-0.0012494234833866358,-0.008483790792524815,-0.057659246027469635,0.052456747740507126,0.002819858258590102,0.024512754753232002,0.013398117385804653,2.085828032825776e-33,0.04113906994462013,-0.012617078609764576,0.04725629836320877,0.05986166000366211,0.055611517280340195,0.061047643423080444,-0.0331895686686039,-0.0509287528693676,0.005364237818866968,-0.05123591423034668,-0.09885791689157486,-0.024326402693986893,-0.04210563004016876,0.09361722320318222,0.034620076417922974,-0.04700815677642822,-0.019558647647500038,-0.004489181563258171,0.06946379691362381,-0.015052126720547676,0.01490260474383831,-0.005963976960629225,0.06774003803730011,0.018073227256536484,0.03015805035829544,0.0932580903172493,0.0601162351667881,-0.10327634960412979,0.0024773210752755404,0.011198539286851883,-0.03773455694317818,0.04291486367583275,-0.039349086582660675,0.028116334229707718,-0.013339336961507797,-0.0005703704664483666,0.009549316018819809,-0.03537015616893768,-0.00478324806317687,0.05166708305478096,-0.029857872053980827,0.01445637084543705,0.010965852998197079,-0.06920788437128067,-0.04060143977403641,-0.008540348149836063,-0.013369369320571423,0.021698519587516785,-0.01275607943534851,-0.020262086763978004,-0.061640121042728424,0.05855822563171387,-0.03336353972554207,-0.00021914263197686523,0.06686099618673325,-0.11709536612033844,0.014179245568811893,0.030882546678185463,0.026584047824144363,0.03593594208359718,-0.028366150334477425,-0.04508542641997337,0.004305346868932247,0.029585670679807663,0.06870269030332565,0.018912170082330704,0.025405043736100197,-0.010620697401463985,0.06628459692001343,-0.016228927299380302,0.01834391988813877,0.011721781454980373,-0.04921652004122734,0.00709138298407197,-0.0877230167388916,0.06892422586679459,0.006485505495220423,-0.059741102159023285,0.014209209010004997,0.025274911895394325,-0.061379607766866684,-0.031035874038934708,-0.01239671092480421,-0.037739790976047516,-0.00006973191921133548,-0.0017952602356672287,0.007961195893585682,-0.04665568843483925,0.02393660694360733,0.0358390137553215,-0.08720207959413528,-0.05086280405521393,-0.01623384840786457,0.024802260100841522,-0.0014483110280707479,-8.396042787500076e-34,-0.08787792921066284,0.051017217338085175,-0.13460621237754822,0.02839367836713791,-0.012305711396038532,-0.061509180814027786,-0.014194165356457233,0.05863112956285477,-0.021025940775871277,0.042561907321214676,-0.019476644694805145,-0.011799189262092113,0.08013126999139786,-0.029417315497994423,0.1023741289973259,-0.05327323451638222,0.01732007972896099,-0.0689525306224823,-0.0013878927566111088,0.007012206595391035,0.005891077686101198,0.035983748733997345,-0.11990314722061157,-0.02372320555150509,0.045067332684993744,0.01407753024250269,-0.02347029186785221,0.031730979681015015,-0.021661745384335518,0.0013510448625311255,0.008465776219964027,-0.006395498290657997,-0.07476705312728882,0.04193492978811264,0.023240096867084503,0.0434027723968029,0.1135043203830719,-0.0075160120613873005,-0.035719726234674454,0.0006876685074530542,0.10927768051624298,-0.0029473404865711927,-0.08059513568878174,-0.031908370554447174,-0.05971018597483635,-0.0031650206074118614,-0.1385878324508667,-0.00011234239354962483,-0.079600989818573,0.002753844251856208,0.060605768114328384,-0.01955392211675644,-0.0016578929498791695,-0.136129230260849,-0.08902304619550705,-0.087124302983284,0.026697825640439987,0.018958622589707375,0.010711593553423882,-0.026872849091887474,-0.05455298721790314,-0.09468193352222443,0.07577286660671234,0.016829170286655426,-0.04537171870470047,-0.031416915357112885,0.022768335416913033,0.08160266280174255,0.037501510232686996,-0.07479515671730042,0.06495421379804611,-0.0793369933962822,0.012775319628417492,0.13848181068897247,-0.01922610029578209,0.029480045661330223,-0.0159646887332201,-0.0007830797112546861,0.04102644696831703,-0.09042316675186157,0.030168859288096428,-0.021151211112737656,0.0621822252869606,0.04709755256772041,0.1419779658317566,0.06341863423585892,0.04736219719052315,0.026672834530472755,0.037960607558488846,0.08311857283115387,-0.05152374878525734,0.08890186250209808,-0.07318367063999176,0.10679275542497635,-0.05496013164520264,-3.451437180501671e-8,-0.06610847264528275,-0.08560970425605774,-0.002760149072855711,0.12190771847963333,0.014594527892768383,-0.029003385454416275,0.011252567172050476,-0.0005150844226591289,-0.015530348755419254,-0.0018444297602400184,0.02225474826991558,-0.0032861491199582815,-0.03525910899043083,-0.05672745779156685,0.048057638108730316,0.06513950973749161,0.01489434577524662,-0.020212160423398018,0.03246872499585152,-0.08314327150583267,0.07683968544006348,-0.024239078164100647,-0.016005169600248337,0.062447402626276016,-0.011879382655024529,-0.05930088832974434,-0.07979603856801987,0.05682040750980377,-0.09436574578285217,0.03901633620262146,0.04745694622397423,-0.016938820481300354,0.004942241590470076,-0.017586225643754005,0.08069387823343277,0.06611203402280807,-0.029947267845273018,-0.07736211270093918,0.004713412374258041,-0.020543068647384644,0.019867584109306335,0.002722677541896701,-0.018550798296928406,-0.06785906851291656,-0.0035530386958271265,-0.06059471517801285,-0.004834994673728943,-0.22411774098873138,0.011943123303353786,-0.03501773625612259,-0.057571105659008026,0.002933186711743474,0.008182323537766933,0.016445664688944817,0.04563618451356888,-0.036417778581380844,0.04033747315406799,-0.011212554760277271,-0.001970109296962619,0.0798109695315361,-0.016713660210371017,0.1386975347995758,0.04442412778735161,-0.06312142312526703]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>[0.049846697598695755,0.00397887360304594,-0.0578894168138504,0.045408476144075394,0.01096608117222786,0.028079262003302574,0.08962110430002213,0.0018600642215460539,-0.09989113360643387,-0.0019044951768592,0.02134629711508751,0.06728007644414902,-0.023504650220274925,-0.02995956502854824,0.053131602704524994,0.01623518206179142,0.04568273946642876,-0.0023787072859704494,-0.024888617917895317,-0.01952662318944931,-0.005630624480545521,0.05725718289613724,0.017260726541280746,0.049985047429800034,-0.03780241683125496,0.01274261437356472,-0.02875550091266632,-0.16248296201229095,-0.02421743795275688,0.03564470633864403,0.06217227131128311,-0.03227050602436066,0.11277730017900467,0.01240825280547142,-0.05530334264039993,0.039943356066942215,0.03207090124487877,0.06292498856782913,-0.02574790082871914,0.049289148300886154,-0.01498825941234827,-0.03427701070904732,0.004209056496620178,-0.000979174510575831,-0.006563927978277206,-0.05234377086162567,-0.017201928421854973,-0.06576039642095566,0.003647554200142622,0.022991083562374115,-0.08447191119194031,-0.05746585130691528,0.10066715627908707,-0.03570913150906563,-0.004878862760961056,0.044797834008932114,-0.0011760129127651453,0.04408353939652443,-0.08332903683185577,0.08194006234407425,-0.03074938803911209,-0.015867160633206367,-0.03344012051820755,-0.050226591527462006,0.10134685784578323,0.12965363264083862,0.032594457268714905,-0.05337728187441826,0.0463082492351532,-0.029254883527755737,-0.07532192766666412,-0.02644622139632702,0.023389898240566254,0.002867409260943532,0.05912856012582779,0.013037260621786118,-0.12151942402124405,-0.019204096868634224,0.0811319500207901,-0.08528289198875427,0.0015331138856709003,0.017248021438717842,-0.07400534301996231,0.05992244556546211,0.04387812316417694,-0.048936326056718826,0.017468921840190887,0.0014968104660511017,-0.06349796801805496,-0.028774365782737732,0.03183431178331375,-0.02381250075995922,-0.09619472175836563,-0.016986433416604996,0.07808227092027664,-0.04556601122021675,0.05819982290267944,-0.04282437637448311,-0.045646388083696365,-0.01758793741464615,-0.06212279573082924,0.0835050493478775,0.008571313694119453,0.04438458010554314,-0.026182521134614944,-0.01464113686233759,0.04614584892988205,0.027402736246585846,-0.029315786436200142,-0.017764586955308914,-0.04550164192914963,0.026302391663193703,0.005700898822396994,-0.07409177720546722,0.04659545421600342,-0.0823468416929245,-0.08820467442274094,-0.014809799380600452,-0.013925878331065178,0.02314085327088833,0.018552901223301888,-0.0035444987006485462,0.03649989515542984,0.010317566804587841,0.022606156766414642,0.030699770897626877,-0.08118592202663422,-5.676099929088483e-34,-0.03426399827003479,0.015964746475219727,-0.010499006137251854,0.026953548192977905,0.006164095364511013,0.034017954021692276,-0.025422152131795883,-0.02931355871260166,0.15726003050804138,0.019669756293296814,-0.002522899303585291,-0.029143448919057846,0.04727606475353241,-0.01578584872186184,-0.07918964326381683,-0.003886585822328925,0.02101597562432289,0.1015244722366333,-0.05608087778091431,0.09506355971097946,0.02106560580432415,0.01145031675696373,-0.05140800401568413,0.006602168548852205,-0.04284641146659851,-0.009862760081887245,0.04492396116256714,-0.014685619622468948,0.09452824294567108,0.009929141961038113,0.022317802533507347,-0.03483698517084122,-0.13417457044124603,-0.047121431678533554,-0.028449367731809616,-0.024760283529758453,0.001429651165381074,-0.029323581606149673,-0.02335602231323719,0.004697030410170555,-0.018191657960414886,-0.007418871391564608,0.027325620874762535,0.05913688242435455,-0.07694205641746521,0.0825737863779068,-0.01042773574590683,-0.08487597107887268,-0.0074829598888754845,-0.03956947475671768,0.02980455756187439,0.04076610133051872,-0.0995323657989502,-0.07823594659566879,-0.016460755839943886,0.053260304033756256,0.013135078363120556,-0.04855608195066452,0.03149404376745224,0.0817815363407135,0.14080284535884857,0.027599971741437912,-0.038812026381492615,-0.062098581343889236,-0.06610291451215744,-0.030883288010954857,0.036391861736774445,-0.08734887838363647,0.022230949252843857,0.012247775681316853,0.04611533135175705,-0.007496211677789688,0.05722345784306526,0.07009455561637878,-0.023494960740208626,0.013043675571680069,-0.028815142810344696,-0.055541545152664185,-0.05477972701191902,-0.07149048149585724,0.01625170186161995,-0.08850276470184326,0.000854303187225014,0.01009934488683939,-0.01766352355480194,-0.010179095901548862,-0.05749516561627388,0.05650729313492775,-0.0579923577606678,-0.006242805626243353,-0.04638364538550377,0.021856868639588356,-0.01456624548882246,0.0010526174446567893,-0.06140325218439102,-8.72847901839735e-34,0.025861555710434914,-0.0011220778105780482,0.027813859283924103,-0.07482649385929108,0.03473788872361183,0.05591234192252159,0.01187700591981411,0.04713165760040283,0.05233421549201012,0.05630986765027046,0.02742520160973072,-0.04175728186964989,0.030043138191103935,-0.05065007880330086,-0.02042834460735321,0.07233808189630508,-0.0352695994079113,0.014293731190264225,0.02174742892384529,0.013604597188532352,0.025283729657530785,0.022670919075608253,-0.010407444089651108,-0.0017092123162001371,0.001302620628848672,0.05121181905269623,-0.018874438479542732,0.03300430253148079,0.006667791400104761,0.0021759544033557177,0.01801772601902485,0.0008621669257991016,-0.012816398404538631,-0.05477668717503548,-0.03802989423274994,0.032328296452760696,-0.0013232786441221833,-0.027064278721809387,-0.09880916029214859,-0.025911131873726845,0.012484398670494556,-0.032439474016427994,0.03485378623008728,0.009034281596541405,0.04765331745147705,-0.024144485592842102,-0.07360723614692688,0.041965629905462265,0.011958223767578602,0.07580982893705368,0.09276336431503296,-0.02898484282195568,0.045404668897390366,-0.06441125273704529,-0.04779805615544319,-0.01658014953136444,-0.04597366601228714,-0.07688918709754944,-0.022903865203261375,-0.055577363818883896,0.027322405949234962,-0.034649450331926346,-0.11420495063066483,0.029087767004966736,-0.04046249762177467,-0.02697395347058773,0.07211686670780182,-0.019226688891649246,0.053844474256038666,0.02729051746428013,0.01975415088236332,-0.040531259030103683,0.034792203456163406,0.020945819094777107,0.045020028948783875,-0.027238816022872925,-0.017351491376757622,0.02366122417151928,0.015102679841220379,-0.008769648149609566,-0.022369733080267906,-0.04382087290287018,0.03960423916578293,0.09472054243087769,-0.1220305785536766,0.005319980904459953,0.09491902589797974,0.017159385606646538,0.0037804064340889454,-0.008255494758486748,-0.06214328110218048,0.011882818304002285,-0.11318336427211761,0.016668224707245827,0.07925127446651459,-1.8508881538537025e-8,0.07987760752439499,-0.07197586447000504,0.09067756682634354,0.010506684891879559,0.00535952765494585,-0.008164770901203156,-0.07109468430280685,0.1664259284734726,-0.10188392549753189,-0.01808079145848751,-0.0567314550280571,0.008427556604146957,-0.060506656765937805,-0.0552796795964241,0.004485383629798889,-0.04359233006834984,0.04150230810046196,0.06590135395526886,0.02649436891078949,-0.006741560995578766,0.015158520080149174,0.0059127481654286385,-0.014268073253333569,-0.029835689812898636,-0.02240515872836113,0.017628325149416924,0.05754011869430542,-0.029071226716041565,-0.04960927367210388,-0.05702514946460724,0.059143245220184326,-0.012442526407539845,0.03502323850989342,-0.02403976581990719,0.040423616766929626,-0.12219715118408203,0.03705451637506485,-0.04670357331633568,-0.014390888623893261,0.05135514959692955,-0.031656842678785324,-0.030953332781791687,0.09201988577842712,0.07905883342027664,0.027938826009631157,0.024743707850575447,-0.06654136627912521,-0.04519815370440483,0.07295609265565872,-0.03581300750374794,0.04361407086253166,0.0641440600156784,0.08666760474443436,-0.009984282776713371,-0.07191206514835358,0.12346111238002777,-0.013717170804738998,0.049434345215559006,-0.07404430955648422,0.009328000247478485,0.09582408517599106,0.09897282719612122,0.012058490887284279,-0.019046423956751823]</t>
+  </si>
+  <si>
+    <t>research about ADHD and info from NHS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>[</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="Helvetica Neue"/>
+        <family val="2"/>
+      </rPr>
+      <t>-0.030104659497737885,-0.0981665551662445,0.057555560022592545,-0.055272843688726425,-0.054194383323192596,0.01957692950963974,0.04024806246161461,0.053779006004333496,0.03159649670124054,-0.004817137029021978,0.004814990796148777,-0.0022808783687651157,-0.054225459694862366,0.052382756024599075,0.041544295847415924,-0.03049256093800068,0.036490313708782196,-0.05618828162550926,-0.04734420403838158,-0.11798878759145737,-0.016252903267741203,0.05154042690992355,0.056684210896492004,0.023115528747439384,0.012668237090110779,-0.02119031734764576,0.0028761872090399265,-0.04598909616470337,0.05893292278051376,-0.009032492525875568,0.008966135792434216,0.0942486971616745,0.06397548317909241,0.09510336816310883,-0.05424845218658447,0.06348787248134613,-0.022107165306806564,-0.06069943681359291,0.03056931309401989,0.016083935275673866,-0.04158519580960274,0.004667674656957388,0.03064749948680401,-0.0008844261756166816,0.09645742177963257,-0.08668006211519241,-0.05796873942017555,0.05077220872044563,-0.07146601378917694,0.01964404061436653,-0.11107786744832993,0.007930520921945572,0.026222867891192436,0.09107282012701035,0.008846708573400974,-0.03436857834458351,-0.019772425293922424,0.04473254457116127,0.013327209278941154,-0.05790960043668747,-0.06239067390561104,-0.03599496930837631,-0.07386906445026398,-0.008800568990409374,-0.026933690533041954,0.04898105934262276,0.009506464935839176,0.06979905068874359,0.037613335996866226,0.0466899573802948,-0.01927596889436245,-0.008842295967042446,-0.046322908252477646,0.07813064754009247,0.0016931374557316303,0.039738044142723083,0.01772945001721382,-0.010685763321816921,0.012844606302678585,-0.02666311524808407,0.029359037056565285,-0.0027254491578787565,0.08777536451816559,-0.07272566109895706,0.006912858225405216,-0.06732599437236786,0.03359042480587959,0.02788035199046135,0.0022054093424230814,0.004019983112812042,-0.035129986703395844,-0.01662558875977993,0.07272212207317352,0.07357468456029892,-0.03259418532252312,-0.0006890423828735948,0.03661135956645012,-0.006830986589193344,-0.0133417509496212,0.09779975563287735,0.008805057033896446,0.05105127766728401,0.04696003720164299,-0.043830692768096924,-0.0281338132917881,-0.03387889266014099,0.003434573533013463,0.014663168229162693,0.018086565658450127,-0.09565971791744232,-0.07479245215654373,-0.008317885920405388,-0.020284367725253105,0.05876398831605911,0.04265547916293144,-0.032088503241539,0.046660684049129486,-0.05230654776096344,-0.0042428248561918736,0.054272763431072235,-0.016619110479950905,0.0033882595598697662,0.0036398873198777437,-0.005885799415409565,-0.04657081514596939,0.047931455075740814,-0.035753555595874786,-1.5414268442592195e-33,0.1000106930732727,0.022367745637893677,-0.03336024656891823,0.09429124742746353,0.007267815992236137,0.0799993947148323,0.014665747992694378,-0.009831724688410759,-0.00982807669788599,-0.08662045001983643,-0.0018427754985168576,-0.018746942281723022,-0.014951555989682674,0.019102493301033974,0.034896500408649445,0.014212802983820438,-0.02153381146490574,0.06811726093292236,0.03960618004202843,-0.02606426551938057,0.028788169845938683,0.06423371285200119,0.007051476277410984,0.0037207372952252626,0.05099833011627197,0.06865327805280685,0.06100013852119446,-0.1008254736661911,-0.04165370762348175,0.04551785811781883,-0.05558013543486595,-0.030864253640174866,-0.01802906021475792,0.036945145577192307,0.05697830393910408,-0.0417601577937603,0.002602790482342243,-0.12798623740673065,0.03732272610068321,-0.08800912648439407,-0.016818571835756302,-0.011204756796360016,0.0053583839908242226,-0.08743687719106674,-0.030739085748791695,0.00614166958257556,-0.017468402162194252,-0.0375397764146328,-0.03380605950951576,0.022574225440621376,0.025532525032758713,0.008076164871454239,-0.03413902595639229,0.05032564699649811,0.018814560025930405,-0.014279771596193314,0.020928559824824333,0.03198217228055,0.04117893427610397,0.10048745572566986,0.006111948285251856,-0.039514631032943726,0.07165708392858505,0.0034674464259296656,0.1193179190158844,-0.0036526708863675594,-0.17198209464550018,-0.028413688763976097,0.07259175181388855,-0.013248324394226074,0.014990042895078659,-0.010931868106126785,0.03507129102945328,0.03576260060071945,-0.04838251695036888,-0.010846412740647793,0.04654296860098839,-0.011611212976276875,0.001457599806599319,0.049388837069272995,-0.09561768174171448,-0.02089516632258892,0.02289672940969467,-0.07911226153373718,-0.00669886963441968,-0.06339288502931595,0.05659504979848862,-0.04841708019375801,-0.004852668382227421,0.03430946543812752,-0.11079999059438705,0.006682853680104017,0.012774557806551456,-0.024397995322942734,0.028644798323512077,1.5305976025522692e-33,-0.04843660444021225,0.05373740196228027,-0.063873790204525,0.03234052285552025,-0.034787602722644806,-0.12253573536872864,0.05685177445411682,0.0969228595495224,-0.023725366219878197,-0.00999075174331665,0.023750850930809975,-0.08045267313718796,0.09449607878923416,-0.04053911566734314,0.1088046282529831,-0.06728701293468475,0.12160316109657288,-0.0764690488576889,0.05705609545111656,0.08378977328538895,0.00012783033889718354,-0.02735080197453499,-0.14318536221981049,0.02287456952035427,0.027868924662470818,0.02598618157207966,-0.07105589658021927,-0.013942530378699303,-0.035848867148160934,0.012827201746404171,-0.0017092747148126364,0.0074353450909256935,-0.07564493268728256,0.03332824632525444,-0.03531346842646599,0.011350140906870365,0.09860958158969879,0.052393462508916855,-0.056001681834459305,0.045906033366918564,0.06836508959531784,-0.06404765695333481,-0.10640022903680801,-0.05162562429904938,0.02737002819776535,0.02986535057425499,-0.1275675743818283,-0.014544637873768806,-0.04560795798897743,-0.02821563556790352,0.04855974391102791,-0.008997827768325806,0.08762595802545547,-0.04528758302330971,-0.006506796460598707,-0.06619558483362198,0.024066362529993057,-0.03805248439311981,-0.03560452163219452,-0.040608324110507965,-0.023267555981874466,-0.05470253527164459,0.07588246464729309,-0.012993764132261276,-0.004196529276669025,-0.09251299500465393,-0.03072298690676689,-0.031836990267038345,0.10686489939689636,-0.02644197829067707,0.038700174540281296,-0.02565186843276024,-0.04574044421315193,0.12024406343698502,-0.012307798489928246,0.0009059582371264696,-0.02344684675335884,-0.01855611801147461,0.06850362569093704,-0.03492823243141174,-0.011297744698822498,0.05638401210308075,0.07328946143388748,0.0076240901835262775,0.1055554524064064,0.03095630183815956,0.03143630921840668,0.07113659381866455,0.028277888894081116,0.027639325708150864,-0.012047147378325462,0.057287707924842834,0.005761364009231329,0.07109423726797104,0.004459819756448269,-1.3889904337816006e-8,-0.045772943645715714,-0.05156349763274193,-0.021357975900173187,0.08875486999750137,-0.0003374664520379156,-0.04643974080681801,-0.04588451236486435,0.027223480865359306,0.01704924739897251,0.10908520221710205,-0.013569425791501999,-0.00031865682103671134,-0.04007415845990181,-0.024375297129154205,-0.005658015608787537,0.0156224574893713,-0.050978582352399826,-0.0028265323489904404,-0.03958786651492119,0.04470546543598175,0.06211285665631294,0.042391207069158554,0.0021093590185046196,0.09707049280405045,0.018736304715275764,-0.0063963825814425945,-0.024969950318336487,0.08845097571611404,-0.024593589827418327,0.001149594783782959,-0.0023895399644970894,0.009353089146316051,-0.07925441861152649,0.010389511473476887,0.03313857316970825,-0.034665413200855255,-0.03943934291601181,-0.024543993175029755,0.02483578398823738,0.016032181680202484,0.08452310413122177,-0.021495340391993523,-0.09035138785839081,0.004151507746428251,0.12005901336669922,-0.030519699677824974,-0.07163219898939133,-0.10899452120065689,-0.00030724593671038747,-0.016731366515159607,-0.05967221036553383,0.04462208226323128,-0.05464881286025047,0.016293631866574287,0.06749425083398819,0.01717185229063034,-0.0018828081665560603,0.011218341998755932,0.0179743655025959,-0.004488683305680752,-0.06055471673607826,0.04590313509106636,-0.010529875755310059,-0.02599893882870674</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="13"/>
+        <color theme="1"/>
+        <rFont val="PingFang SC"/>
+        <family val="2"/>
+        <charset val="134"/>
+      </rPr>
+      <t>]</t>
+    </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -3723,7 +3755,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="13">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -3798,6 +3830,26 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="DengXian"/>
+      <family val="4"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="13"/>
+      <color theme="1"/>
+      <name val="PingFang SC"/>
+      <family val="2"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -3824,7 +3876,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3838,6 +3890,12 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4286,8 +4344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B65D772C-AA75-AA43-9504-F09D4F1E798F}">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4335,13 +4393,13 @@
         <v>20</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>21</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="172" customHeight="1">
@@ -4355,13 +4413,13 @@
         <v>22</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>23</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="206" customHeight="1">
@@ -4375,13 +4433,13 @@
         <v>26</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>27</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="223" customHeight="1">
@@ -4395,13 +4453,13 @@
         <v>24</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>25</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="409.6">
@@ -4415,13 +4473,13 @@
         <v>28</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>29</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="359" customHeight="1">
@@ -4432,56 +4490,56 @@
         <v>30</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="F7" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="282" customHeight="1">
       <c r="A8" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="B8" s="2" t="s">
         <v>32</v>
       </c>
+      <c r="B8" s="3" t="s">
+        <v>59</v>
+      </c>
       <c r="C8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>45</v>
-      </c>
       <c r="G8" s="2" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="323" customHeight="1">
       <c r="A9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="F9" s="2" t="s">
+      <c r="G9" s="2" t="s">
         <v>37</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -4489,6 +4547,7 @@
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" location="module_pipelines.FeatureExtractionPipeline" xr:uid="{11082AA2-1362-C843-A16F-47E3992BA907}"/>
     <hyperlink ref="B6" r:id="rId2" xr:uid="{FD673EAC-FB42-4D4D-B4AF-788C700A37BA}"/>
+    <hyperlink ref="B8" r:id="rId3" xr:uid="{C99D7C29-2DDC-2347-85CC-19A0E59EC84F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -4497,10 +4556,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B1569DC-67C3-7942-A37B-0CCAFF34F563}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -4512,15 +4571,26 @@
   <sheetData>
     <row r="1" spans="1:2" ht="52" customHeight="1">
       <c r="A1" s="4" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="17">
+    <row r="2" spans="1:2" ht="409.6">
       <c r="A2" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="409.6">
+      <c r="A3" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>

</xml_diff>